<commit_message>
updated code, excel spreadshhjet and document
</commit_message>
<xml_diff>
--- a/Exercises/baker.xlsx
+++ b/Exercises/baker.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/UT-Causal-Inference/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B880C5-E4EE-3744-B4F0-923BC39D1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73998339-B2EF-8A49-81BF-D6D25D052D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="50180" windowHeight="28240" xr2:uid="{240EE8BD-E578-F640-BA93-D22B7313B1B2}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="50180" windowHeight="28240" activeTab="1" xr2:uid="{240EE8BD-E578-F640-BA93-D22B7313B1B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dynamic TE" sheetId="1" r:id="rId1"/>
+    <sheet name="constant TE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="83">
   <si>
     <t>Year</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Group 4 (treated in 2004)</t>
   </si>
   <si>
-    <t>Each cell is a group-time ATT(g,t)</t>
-  </si>
-  <si>
     <t>Number of post-treatment ATT(g,t)</t>
   </si>
   <si>
@@ -74,15 +72,9 @@
     <t>1.Why do I have two different overall ATT measures?</t>
   </si>
   <si>
-    <t>weights</t>
-  </si>
-  <si>
     <t>uniformly weighting each ATT(g,t) -- 1/60</t>
   </si>
   <si>
-    <t>these weights are a little more complex</t>
-  </si>
-  <si>
     <t>first, sum and divide by total number of</t>
   </si>
   <si>
@@ -221,9 +213,6 @@
     <t>Number possible</t>
   </si>
   <si>
-    <t>Feasible ATT</t>
-  </si>
-  <si>
     <t>Can we identify this ATT(g,t)?</t>
   </si>
   <si>
@@ -236,9 +225,6 @@
     <t>36 ATT(g,t) bc we can't use the post 2004</t>
   </si>
   <si>
-    <t>ATT(g)-hat</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -267,13 +253,43 @@
   </si>
   <si>
     <t>But as Scott, if we had a fifth group who was "never treated", we'd get all 60</t>
+  </si>
+  <si>
+    <t>True ATTs are weighted averages over all ATT(g,t)</t>
+  </si>
+  <si>
+    <t>Weighted average over all group-time ATT(g,t)</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>weights of 1/4 per ATT(g), but that ATT(g) had been based on different weighting</t>
+  </si>
+  <si>
+    <t>N with CS</t>
+  </si>
+  <si>
+    <t>ATT(g) w/ CS</t>
+  </si>
+  <si>
+    <t>ATT w/ CS</t>
+  </si>
+  <si>
+    <t>Total cells</t>
+  </si>
+  <si>
+    <t>CS cells</t>
+  </si>
+  <si>
+    <t>Number of cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,8 +311,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +363,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -422,21 +458,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,10 +602,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,45 +962,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C99536-70B7-CD46-A942-EAD2AFA2EFA9}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="12.5" style="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.5" style="1"/>
     <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
     <col min="10" max="10" width="41.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
+      <c r="I1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -862,12 +1028,7 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1">
-        <v>60</v>
-      </c>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -886,17 +1047,18 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="G3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16">
+        <f>AVERAGE(B8:B31,C14:C31,D20:D31,E26:E31)</f>
         <v>82</v>
       </c>
-      <c r="J3" s="19" t="s">
-        <v>14</v>
+      <c r="J3" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -915,14 +1077,14 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>9</v>
+      <c r="H4" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1983</v>
       </c>
@@ -938,17 +1100,18 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="21">
+      <c r="H5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="18">
+        <f>AVERAGE(B33:E33)</f>
         <v>63.5</v>
       </c>
-      <c r="J5" s="21" t="s">
-        <v>15</v>
+      <c r="J5" s="32" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -968,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -988,20 +1151,20 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H7" s="1">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1986</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="2">
         <v>10</v>
       </c>
       <c r="C8" s="1">
@@ -1014,23 +1177,23 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="22">
+        <v>37</v>
+      </c>
+      <c r="H8" s="19">
         <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1987</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>20</v>
       </c>
       <c r="C9" s="1">
@@ -1043,23 +1206,23 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="22">
+        <v>38</v>
+      </c>
+      <c r="H9" s="19">
         <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1988</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>30</v>
       </c>
       <c r="C10" s="1">
@@ -1072,17 +1235,17 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1989</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>40</v>
       </c>
       <c r="C11" s="1">
@@ -1095,23 +1258,23 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1990</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>50</v>
       </c>
       <c r="C12" s="1">
@@ -1124,23 +1287,23 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1991</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>60</v>
       </c>
       <c r="C13" s="1">
@@ -1153,26 +1316,26 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1992</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>70</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>8</v>
       </c>
       <c r="D14" s="1">
@@ -1182,23 +1345,23 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1993</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>80</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6">
         <v>16</v>
       </c>
       <c r="D15" s="1">
@@ -1208,20 +1371,20 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1994</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>90</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="6">
         <v>24</v>
       </c>
       <c r="D16" s="1">
@@ -1231,23 +1394,23 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1995</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>100</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="6">
         <v>32</v>
       </c>
       <c r="D17" s="1">
@@ -1257,23 +1420,23 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1996</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>110</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="6">
         <v>40</v>
       </c>
       <c r="D18" s="1">
@@ -1283,23 +1446,23 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1997</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="3">
         <v>120</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <v>48</v>
       </c>
       <c r="D19" s="1">
@@ -1309,397 +1472,1310 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1998</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>130</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="6">
         <v>56</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1999</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>140</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <v>64</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="9">
         <v>12</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2000</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>150</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="6">
         <v>72</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="9">
         <v>18</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2001</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="3">
         <v>160</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="6">
         <v>80</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2002</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>170</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="6">
         <v>88</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="9">
         <v>30</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2003</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="3">
         <v>180</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="6">
         <v>96</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="9">
         <v>36</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2004</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>190</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="6">
         <v>104</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>42</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="11">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>66</v>
+      <c r="G26" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2005</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="3">
         <v>200</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="6">
         <v>112</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="9">
         <v>48</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="12">
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2006</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="3">
         <v>210</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="6">
         <v>120</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="9">
         <v>54</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="12">
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="17">
+        <v>61</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="40">
         <f>AVERAGE(D20:D25,C14:C25,B8:B25)</f>
         <v>68.333333333333329</v>
       </c>
       <c r="J28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2007</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="3">
         <v>220</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="6">
         <v>128</v>
       </c>
-      <c r="D29" s="12">
-        <v>60</v>
-      </c>
-      <c r="E29" s="15">
+      <c r="D29" s="9">
+        <v>60</v>
+      </c>
+      <c r="E29" s="12">
         <v>16</v>
       </c>
       <c r="F29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
         <v>65</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2008</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="3">
         <v>230</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="6">
         <v>136</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="9">
         <v>66</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="12">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="H30" s="17">
-        <f>AVERAGE(B34:D34)</f>
+        <v>61</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="14">
+        <f>AVERAGE(B36:D36)</f>
         <v>56</v>
       </c>
       <c r="J30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2009</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="4">
         <v>240</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="7">
         <v>144</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <v>72</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="13">
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="29">
+        <f>AVERAGE(B8:B31)</f>
+        <v>125</v>
+      </c>
+      <c r="C33" s="29">
+        <f>AVERAGE(C14:C31)</f>
+        <v>76</v>
+      </c>
+      <c r="D33" s="29">
+        <f>AVERAGE(D20:D31)</f>
         <v>39</v>
       </c>
-      <c r="J32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="1">
-        <v>125</v>
-      </c>
-      <c r="C33" s="1">
-        <v>76</v>
-      </c>
-      <c r="D33" s="1">
-        <v>39</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="E33" s="30">
+        <f>AVERAGE(E26:E31)</f>
         <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="31" t="str">
+        <f>"1/24"</f>
+        <v>1/24</v>
+      </c>
+      <c r="C34" s="29" t="str">
+        <f>"1/18"</f>
+        <v>1/18</v>
+      </c>
+      <c r="D34" s="29" t="str">
+        <f>"1/12"</f>
+        <v>1/12</v>
+      </c>
+      <c r="E34" s="30" t="str">
+        <f>"1/6"</f>
+        <v>1/6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="34" t="str">
+        <f>"18"</f>
+        <v>18</v>
+      </c>
+      <c r="C35" s="35" t="str">
+        <f>"12"</f>
+        <v>12</v>
+      </c>
+      <c r="D35" s="35" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="38">
         <f>AVERAGE(B8:B25)</f>
         <v>95</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C36" s="38">
         <f>AVERAGE(C14:C25)</f>
         <v>52</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D36" s="38">
         <f>AVERAGE(D20:D25)</f>
         <v>21</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E36" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1">
+        <v>60</v>
+      </c>
+      <c r="J38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="1">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD78860-C563-F14A-8DA4-71BC28A5B654}">
+  <dimension ref="A1:K39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.5" style="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="41.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1980</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1981</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16" t="e">
+        <f>AVERAGE(B8:B31,C14:C31,D20:D31,E26:E31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1982</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1983</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="18" t="e">
+        <f>AVERAGE(B33:E33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1984</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1985</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1986</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="19">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1987</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="19">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1988</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1989</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1990</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1991</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1992</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1993</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1994</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1995</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1996</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1997</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1998</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1999</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2000</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2002</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2003</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2004</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="11"/>
+      <c r="F26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2005</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="12"/>
+      <c r="F27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2006</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="12"/>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="40" t="e">
+        <f>AVERAGE(D20:D25,C14:C25,B8:B25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2007</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="12"/>
+      <c r="F29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2008</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12"/>
+      <c r="F30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="14" t="e">
+        <f>AVERAGE(B36:D36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2009</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="F31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
         <v>68</v>
       </c>
-      <c r="J34" t="s">
+    </row>
+    <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="29" t="e">
+        <f>AVERAGE(B8:B31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C33" s="29" t="e">
+        <f>AVERAGE(C14:C31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D33" s="29" t="e">
+        <f>AVERAGE(D20:D31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" s="30" t="e">
+        <f>AVERAGE(E26:E31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
         <v>75</v>
       </c>
+      <c r="B34" s="31" t="str">
+        <f>"1/24"</f>
+        <v>1/24</v>
+      </c>
+      <c r="C34" s="29" t="str">
+        <f>"1/18"</f>
+        <v>1/18</v>
+      </c>
+      <c r="D34" s="29" t="str">
+        <f>"1/12"</f>
+        <v>1/12</v>
+      </c>
+      <c r="E34" s="30" t="str">
+        <f>"1/6"</f>
+        <v>1/6</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="34" t="str">
+        <f>"18"</f>
+        <v>18</v>
+      </c>
+      <c r="C35" s="35" t="str">
+        <f>"12"</f>
+        <v>12</v>
+      </c>
+      <c r="D35" s="35" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>63</v>
+      </c>
       <c r="J35" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="38" t="e">
+        <f>AVERAGE(B8:B25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C36" s="38" t="e">
+        <f>AVERAGE(C14:C25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D36" s="38" t="e">
+        <f>AVERAGE(D20:D25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J37" t="s">
-        <v>77</v>
+      <c r="B37" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1">
+        <v>60</v>
+      </c>
+      <c r="J38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="1">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>